<commit_message>
Fix dms to dd conversion and fix erroneous coordinates in buoy data
</commit_message>
<xml_diff>
--- a/data/buoys/Buoys_2023_04_01.xlsx
+++ b/data/buoys/Buoys_2023_04_01.xlsx
@@ -1034,9 +1034,6 @@
     <t>22BS-5A</t>
   </si>
   <si>
-    <t>59°54.747’W, 171°43.379’W</t>
-  </si>
-  <si>
     <t>46 feet</t>
   </si>
   <si>
@@ -2607,6 +2604,9 @@
   </si>
   <si>
     <t>TYPE.NAME</t>
+  </si>
+  <si>
+    <t>59°54.747'N, 171°43.379’W</t>
   </si>
 </sst>
 </file>
@@ -2928,7 +2928,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J254"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2942,7 +2944,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="B1" t="s">
         <v>83</v>
@@ -4705,13 +4707,13 @@
         <v>335</v>
       </c>
       <c r="B89" t="s">
-        <v>336</v>
+        <v>860</v>
       </c>
       <c r="C89" t="s">
         <v>318</v>
       </c>
       <c r="D89" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>324</v>
@@ -4722,16 +4724,16 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
+        <v>337</v>
+      </c>
+      <c r="B90" t="s">
         <v>338</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
         <v>339</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D90" t="s">
         <v>340</v>
-      </c>
-      <c r="D90" t="s">
-        <v>341</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>324</v>
@@ -4742,16 +4744,16 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
+        <v>341</v>
+      </c>
+      <c r="B91" t="s">
         <v>342</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" t="s">
         <v>343</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
         <v>344</v>
-      </c>
-      <c r="D91" t="s">
-        <v>345</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>324</v>
@@ -4762,13 +4764,13 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
+        <v>345</v>
+      </c>
+      <c r="B92" t="s">
         <v>346</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
         <v>347</v>
-      </c>
-      <c r="C92" t="s">
-        <v>348</v>
       </c>
       <c r="D92" t="s">
         <v>271</v>
@@ -4782,13 +4784,13 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
+        <v>348</v>
+      </c>
+      <c r="B93" t="s">
         <v>349</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" t="s">
         <v>350</v>
-      </c>
-      <c r="C93" t="s">
-        <v>351</v>
       </c>
       <c r="D93" t="s">
         <v>318</v>
@@ -4802,10 +4804,10 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
+        <v>351</v>
+      </c>
+      <c r="B94" t="s">
         <v>352</v>
-      </c>
-      <c r="B94" t="s">
-        <v>353</v>
       </c>
       <c r="C94" t="s">
         <v>179</v>
@@ -4822,19 +4824,19 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
+        <v>353</v>
+      </c>
+      <c r="B95" t="s">
         <v>354</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" t="s">
         <v>355</v>
       </c>
-      <c r="C95" t="s">
+      <c r="D95" t="s">
         <v>356</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E95" s="1" t="s">
         <v>357</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>358</v>
       </c>
       <c r="F95" t="s">
         <v>46</v>
@@ -4842,16 +4844,16 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
+        <v>358</v>
+      </c>
+      <c r="B96" t="s">
         <v>359</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C96" t="s">
         <v>360</v>
       </c>
-      <c r="C96" t="s">
+      <c r="D96" t="s">
         <v>361</v>
-      </c>
-      <c r="D96" t="s">
-        <v>362</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>301</v>
@@ -4862,59 +4864,59 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
+        <v>362</v>
+      </c>
+      <c r="B97" t="s">
         <v>363</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97" t="s">
         <v>364</v>
       </c>
-      <c r="C97" t="s">
+      <c r="D97" t="s">
         <v>365</v>
       </c>
-      <c r="D97" t="s">
+      <c r="E97" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="E97" s="1" t="s">
+      <c r="F97" t="s">
         <v>367</v>
-      </c>
-      <c r="F97" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
+        <v>368</v>
+      </c>
+      <c r="B98" t="s">
         <v>369</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" t="s">
         <v>370</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D98" t="s">
         <v>371</v>
       </c>
-      <c r="D98" t="s">
-        <v>372</v>
-      </c>
       <c r="E98" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="F98" t="s">
         <v>367</v>
-      </c>
-      <c r="F98" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
+        <v>372</v>
+      </c>
+      <c r="B99" t="s">
         <v>373</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" t="s">
         <v>374</v>
       </c>
-      <c r="C99" t="s">
+      <c r="D99" t="s">
         <v>375</v>
       </c>
-      <c r="D99" t="s">
+      <c r="E99" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>377</v>
       </c>
       <c r="F99" t="s">
         <v>167</v>
@@ -4922,16 +4924,16 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
+        <v>377</v>
+      </c>
+      <c r="B100" t="s">
         <v>378</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C100" t="s">
         <v>379</v>
       </c>
-      <c r="C100" t="s">
+      <c r="D100" t="s">
         <v>380</v>
-      </c>
-      <c r="D100" t="s">
-        <v>381</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>315</v>
@@ -4942,19 +4944,19 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
+        <v>381</v>
+      </c>
+      <c r="B101" t="s">
         <v>382</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" t="s">
         <v>383</v>
       </c>
-      <c r="C101" t="s">
+      <c r="D101" t="s">
         <v>384</v>
       </c>
-      <c r="D101" t="s">
-        <v>385</v>
-      </c>
       <c r="E101" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F101" t="s">
         <v>167</v>
@@ -4962,19 +4964,19 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
+        <v>385</v>
+      </c>
+      <c r="B102" t="s">
         <v>386</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" t="s">
+        <v>375</v>
+      </c>
+      <c r="D102" t="s">
         <v>387</v>
       </c>
-      <c r="C102" t="s">
+      <c r="E102" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="D102" t="s">
-        <v>388</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>377</v>
       </c>
       <c r="F102" t="s">
         <v>167</v>
@@ -4982,71 +4984,71 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
+        <v>388</v>
+      </c>
+      <c r="B103" t="s">
         <v>389</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103" t="s">
         <v>390</v>
       </c>
-      <c r="C103" t="s">
+      <c r="D103" t="s">
         <v>391</v>
       </c>
-      <c r="D103" t="s">
+      <c r="E103" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="E103" s="1" t="s">
+      <c r="F103" t="s">
         <v>393</v>
-      </c>
-      <c r="F103" t="s">
-        <v>394</v>
       </c>
       <c r="J103" s="2"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B104" t="s">
+        <v>394</v>
+      </c>
+      <c r="C104" t="s">
         <v>395</v>
       </c>
-      <c r="C104" t="s">
+      <c r="D104" t="s">
         <v>396</v>
       </c>
-      <c r="D104" t="s">
+      <c r="E104" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="F104" t="s">
         <v>397</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="F104" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
+        <v>399</v>
+      </c>
+      <c r="B105" t="s">
         <v>400</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" t="s">
         <v>401</v>
-      </c>
-      <c r="C105" t="s">
-        <v>402</v>
       </c>
       <c r="D105" t="s">
         <v>65</v>
       </c>
       <c r="E105" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="F105" t="s">
         <v>403</v>
-      </c>
-      <c r="F105" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
+        <v>404</v>
+      </c>
+      <c r="B106" t="s">
         <v>405</v>
-      </c>
-      <c r="B106" t="s">
-        <v>406</v>
       </c>
       <c r="C106" t="s">
         <v>133</v>
@@ -5063,10 +5065,10 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
+        <v>406</v>
+      </c>
+      <c r="B107" t="s">
         <v>407</v>
-      </c>
-      <c r="B107" t="s">
-        <v>408</v>
       </c>
       <c r="C107" t="s">
         <v>133</v>
@@ -5083,79 +5085,79 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
+        <v>408</v>
+      </c>
+      <c r="B108" t="s">
         <v>409</v>
       </c>
-      <c r="B108" t="s">
+      <c r="C108" t="s">
         <v>410</v>
-      </c>
-      <c r="C108" t="s">
-        <v>411</v>
       </c>
       <c r="D108" t="s">
         <v>134</v>
       </c>
       <c r="E108" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="F108" t="s">
         <v>412</v>
-      </c>
-      <c r="F108" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
+        <v>413</v>
+      </c>
+      <c r="B109" t="s">
         <v>414</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" t="s">
+        <v>410</v>
+      </c>
+      <c r="D109" t="s">
         <v>415</v>
       </c>
-      <c r="C109" t="s">
+      <c r="E109" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="D109" t="s">
-        <v>416</v>
-      </c>
-      <c r="E109" s="1" t="s">
+      <c r="F109" t="s">
         <v>412</v>
-      </c>
-      <c r="F109" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
+        <v>416</v>
+      </c>
+      <c r="B110" t="s">
         <v>417</v>
       </c>
-      <c r="B110" t="s">
-        <v>418</v>
-      </c>
       <c r="C110" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D110" t="s">
         <v>134</v>
       </c>
       <c r="E110" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="F110" t="s">
         <v>412</v>
-      </c>
-      <c r="F110" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
+        <v>418</v>
+      </c>
+      <c r="B111" t="s">
         <v>419</v>
-      </c>
-      <c r="B111" t="s">
-        <v>420</v>
       </c>
       <c r="C111" t="s">
         <v>206</v>
       </c>
       <c r="D111" t="s">
+        <v>420</v>
+      </c>
+      <c r="E111" s="1" t="s">
         <v>421</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>422</v>
       </c>
       <c r="F111" t="s">
         <v>167</v>
@@ -5163,10 +5165,10 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
+        <v>422</v>
+      </c>
+      <c r="B112" t="s">
         <v>423</v>
-      </c>
-      <c r="B112" t="s">
-        <v>424</v>
       </c>
       <c r="C112" t="s">
         <v>117</v>
@@ -5175,7 +5177,7 @@
         <v>134</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F112" t="s">
         <v>273</v>
@@ -5183,10 +5185,10 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
+        <v>425</v>
+      </c>
+      <c r="B113" t="s">
         <v>426</v>
-      </c>
-      <c r="B113" t="s">
-        <v>427</v>
       </c>
       <c r="C113" t="s">
         <v>97</v>
@@ -5195,27 +5197,27 @@
         <v>134</v>
       </c>
       <c r="E113" t="s">
+        <v>427</v>
+      </c>
+      <c r="F113" t="s">
         <v>428</v>
-      </c>
-      <c r="F113" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B114" t="s">
+        <v>429</v>
+      </c>
+      <c r="C114" t="s">
         <v>430</v>
-      </c>
-      <c r="C114" t="s">
-        <v>431</v>
       </c>
       <c r="D114" t="s">
         <v>271</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F114" t="s">
         <v>187</v>
@@ -5223,10 +5225,10 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
+        <v>432</v>
+      </c>
+      <c r="B115" t="s">
         <v>433</v>
-      </c>
-      <c r="B115" t="s">
-        <v>434</v>
       </c>
       <c r="C115" t="s">
         <v>184</v>
@@ -5235,178 +5237,178 @@
         <v>174</v>
       </c>
       <c r="E115" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F115" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
+        <v>435</v>
+      </c>
+      <c r="B116" t="s">
         <v>436</v>
       </c>
-      <c r="B116" t="s">
-        <v>437</v>
-      </c>
       <c r="C116" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D116" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E116" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F116" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
+        <v>437</v>
+      </c>
+      <c r="B117" t="s">
         <v>438</v>
       </c>
-      <c r="B117" t="s">
-        <v>439</v>
-      </c>
       <c r="C117" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D117" t="s">
         <v>128</v>
       </c>
       <c r="E117" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F117" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
+        <v>439</v>
+      </c>
+      <c r="B118" t="s">
         <v>440</v>
       </c>
-      <c r="B118" t="s">
-        <v>441</v>
-      </c>
       <c r="C118" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D118" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E118" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F118" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
+        <v>441</v>
+      </c>
+      <c r="B119" t="s">
         <v>442</v>
       </c>
-      <c r="B119" t="s">
-        <v>443</v>
-      </c>
       <c r="C119" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D119" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E119" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F119" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
+        <v>443</v>
+      </c>
+      <c r="B120" t="s">
         <v>444</v>
       </c>
-      <c r="B120" t="s">
-        <v>445</v>
-      </c>
       <c r="C120" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D120" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E120" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F120" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
+        <v>445</v>
+      </c>
+      <c r="B121" t="s">
         <v>446</v>
       </c>
-      <c r="B121" t="s">
-        <v>447</v>
-      </c>
       <c r="C121" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D121" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E121" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F121" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
+        <v>447</v>
+      </c>
+      <c r="B122" t="s">
         <v>448</v>
-      </c>
-      <c r="B122" t="s">
-        <v>449</v>
       </c>
       <c r="C122" t="s">
         <v>313</v>
       </c>
       <c r="D122" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E122" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F122" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
+        <v>449</v>
+      </c>
+      <c r="B123" t="s">
         <v>450</v>
-      </c>
-      <c r="B123" t="s">
-        <v>451</v>
       </c>
       <c r="C123" t="s">
         <v>265</v>
       </c>
       <c r="D123" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E123" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F123" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
+        <v>451</v>
+      </c>
+      <c r="B124" t="s">
         <v>452</v>
-      </c>
-      <c r="B124" t="s">
-        <v>453</v>
       </c>
       <c r="C124" t="s">
         <v>50</v>
@@ -5415,1038 +5417,1038 @@
         <v>92</v>
       </c>
       <c r="E124" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F124" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
+        <v>453</v>
+      </c>
+      <c r="B125" t="s">
         <v>454</v>
       </c>
-      <c r="B125" t="s">
-        <v>455</v>
-      </c>
       <c r="C125" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D125" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="F125" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
+        <v>455</v>
+      </c>
+      <c r="B126" t="s">
         <v>456</v>
       </c>
-      <c r="B126" t="s">
-        <v>457</v>
-      </c>
       <c r="C126" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D126" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="F126" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
+        <v>457</v>
+      </c>
+      <c r="B127" t="s">
         <v>458</v>
       </c>
-      <c r="B127" t="s">
-        <v>459</v>
-      </c>
       <c r="C127" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D127" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="F127" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
+        <v>459</v>
+      </c>
+      <c r="B128" t="s">
         <v>460</v>
       </c>
-      <c r="B128" t="s">
-        <v>461</v>
-      </c>
       <c r="C128" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D128" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="F128" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
+        <v>461</v>
+      </c>
+      <c r="B129" t="s">
         <v>462</v>
       </c>
-      <c r="B129" t="s">
-        <v>463</v>
-      </c>
       <c r="C129" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D129" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="F129" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
+        <v>463</v>
+      </c>
+      <c r="B130" t="s">
         <v>464</v>
       </c>
-      <c r="B130" t="s">
-        <v>465</v>
-      </c>
       <c r="C130" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D130" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="F130" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
+        <v>465</v>
+      </c>
+      <c r="B131" t="s">
         <v>466</v>
       </c>
-      <c r="B131" t="s">
+      <c r="C131" t="s">
+        <v>410</v>
+      </c>
+      <c r="D131" t="s">
+        <v>752</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="F131" t="s">
         <v>467</v>
-      </c>
-      <c r="C131" t="s">
-        <v>411</v>
-      </c>
-      <c r="D131" t="s">
-        <v>753</v>
-      </c>
-      <c r="E131" s="1" t="s">
-        <v>756</v>
-      </c>
-      <c r="F131" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
+        <v>468</v>
+      </c>
+      <c r="B132" t="s">
         <v>469</v>
       </c>
-      <c r="B132" t="s">
-        <v>470</v>
-      </c>
       <c r="C132" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D132" t="s">
         <v>271</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F132" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
+        <v>470</v>
+      </c>
+      <c r="B133" t="s">
         <v>471</v>
       </c>
-      <c r="B133" t="s">
-        <v>472</v>
-      </c>
       <c r="C133" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="D133" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F133" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
+        <v>472</v>
+      </c>
+      <c r="B134" t="s">
         <v>473</v>
       </c>
-      <c r="B134" t="s">
-        <v>474</v>
-      </c>
       <c r="C134" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="D134" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F134" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
+        <v>474</v>
+      </c>
+      <c r="B135" t="s">
         <v>475</v>
       </c>
-      <c r="B135" t="s">
-        <v>476</v>
-      </c>
       <c r="C135" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D135" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F135" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
+        <v>476</v>
+      </c>
+      <c r="B136" t="s">
         <v>477</v>
       </c>
-      <c r="B136" t="s">
-        <v>478</v>
-      </c>
       <c r="C136" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D136" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F136" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
+        <v>478</v>
+      </c>
+      <c r="B137" t="s">
         <v>479</v>
       </c>
-      <c r="B137" t="s">
-        <v>480</v>
-      </c>
       <c r="C137" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D137" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F137" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
+        <v>480</v>
+      </c>
+      <c r="B138" t="s">
         <v>481</v>
       </c>
-      <c r="B138" t="s">
-        <v>482</v>
-      </c>
       <c r="C138" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D138" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F138" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
+        <v>482</v>
+      </c>
+      <c r="B139" t="s">
         <v>483</v>
       </c>
-      <c r="B139" t="s">
-        <v>484</v>
-      </c>
       <c r="C139" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D139" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F139" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
+        <v>484</v>
+      </c>
+      <c r="B140" t="s">
         <v>485</v>
       </c>
-      <c r="B140" t="s">
-        <v>486</v>
-      </c>
       <c r="C140" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D140" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F140" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
+        <v>486</v>
+      </c>
+      <c r="B141" t="s">
         <v>487</v>
       </c>
-      <c r="B141" t="s">
-        <v>488</v>
-      </c>
       <c r="C141" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D141" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F141" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
+        <v>488</v>
+      </c>
+      <c r="B142" t="s">
         <v>489</v>
       </c>
-      <c r="B142" t="s">
-        <v>490</v>
-      </c>
       <c r="C142" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="D142" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F142" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
+        <v>490</v>
+      </c>
+      <c r="B143" t="s">
         <v>491</v>
       </c>
-      <c r="B143" t="s">
-        <v>492</v>
-      </c>
       <c r="C143" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="D143" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F143" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
+        <v>492</v>
+      </c>
+      <c r="B144" t="s">
         <v>493</v>
       </c>
-      <c r="B144" t="s">
-        <v>494</v>
-      </c>
       <c r="C144" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D144" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F144" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
+        <v>494</v>
+      </c>
+      <c r="B145" t="s">
         <v>495</v>
       </c>
-      <c r="B145" t="s">
-        <v>496</v>
-      </c>
       <c r="C145" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D145" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F145" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
+        <v>496</v>
+      </c>
+      <c r="B146" t="s">
         <v>497</v>
       </c>
-      <c r="B146" t="s">
-        <v>498</v>
-      </c>
       <c r="C146" t="s">
+        <v>582</v>
+      </c>
+      <c r="D146" t="s">
         <v>583</v>
       </c>
-      <c r="D146" t="s">
-        <v>584</v>
-      </c>
       <c r="E146" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F146" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
+        <v>498</v>
+      </c>
+      <c r="B147" t="s">
         <v>499</v>
       </c>
-      <c r="B147" t="s">
-        <v>500</v>
-      </c>
       <c r="C147" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="D147" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F147" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
+        <v>500</v>
+      </c>
+      <c r="B148" t="s">
         <v>501</v>
       </c>
-      <c r="B148" t="s">
-        <v>502</v>
-      </c>
       <c r="C148" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D148" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F148" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
+        <v>502</v>
+      </c>
+      <c r="B149" t="s">
         <v>503</v>
       </c>
-      <c r="B149" t="s">
+      <c r="C149" t="s">
         <v>504</v>
       </c>
-      <c r="C149" t="s">
+      <c r="D149" t="s">
         <v>505</v>
       </c>
-      <c r="D149" t="s">
+      <c r="E149" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="E149" s="1" t="s">
-        <v>507</v>
-      </c>
       <c r="F149" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
+        <v>507</v>
+      </c>
+      <c r="B150" t="s">
         <v>508</v>
-      </c>
-      <c r="B150" t="s">
-        <v>509</v>
       </c>
       <c r="C150" t="s">
         <v>16</v>
       </c>
       <c r="D150" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F150" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
+        <v>510</v>
+      </c>
+      <c r="B151" t="s">
         <v>511</v>
-      </c>
-      <c r="B151" t="s">
-        <v>512</v>
       </c>
       <c r="C151" t="s">
         <v>21</v>
       </c>
       <c r="D151" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F151" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
+        <v>513</v>
+      </c>
+      <c r="B152" t="s">
         <v>514</v>
       </c>
-      <c r="B152" t="s">
+      <c r="C152" t="s">
         <v>515</v>
       </c>
-      <c r="C152" t="s">
+      <c r="D152" t="s">
         <v>516</v>
       </c>
-      <c r="D152" t="s">
-        <v>517</v>
-      </c>
       <c r="E152" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F152" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
+        <v>517</v>
+      </c>
+      <c r="B153" t="s">
         <v>518</v>
       </c>
-      <c r="B153" t="s">
+      <c r="C153" t="s">
         <v>519</v>
       </c>
-      <c r="C153" t="s">
+      <c r="D153" t="s">
         <v>520</v>
       </c>
-      <c r="D153" t="s">
-        <v>521</v>
-      </c>
       <c r="E153" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F153" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
+        <v>521</v>
+      </c>
+      <c r="B154" t="s">
         <v>522</v>
       </c>
-      <c r="B154" t="s">
+      <c r="C154" t="s">
         <v>523</v>
       </c>
-      <c r="C154" t="s">
+      <c r="D154" t="s">
         <v>524</v>
       </c>
-      <c r="D154" t="s">
-        <v>525</v>
-      </c>
       <c r="E154" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F154" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
+        <v>525</v>
+      </c>
+      <c r="B155" t="s">
         <v>526</v>
       </c>
-      <c r="B155" t="s">
+      <c r="C155" t="s">
         <v>527</v>
       </c>
-      <c r="C155" t="s">
+      <c r="D155" t="s">
         <v>528</v>
       </c>
-      <c r="D155" t="s">
-        <v>529</v>
-      </c>
       <c r="E155" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F155" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
+        <v>529</v>
+      </c>
+      <c r="B156" t="s">
         <v>530</v>
       </c>
-      <c r="B156" t="s">
+      <c r="C156" t="s">
         <v>531</v>
       </c>
-      <c r="C156" t="s">
+      <c r="D156" t="s">
         <v>532</v>
       </c>
-      <c r="D156" t="s">
-        <v>533</v>
-      </c>
       <c r="E156" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F156" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
+        <v>533</v>
+      </c>
+      <c r="B157" t="s">
         <v>534</v>
       </c>
-      <c r="B157" t="s">
+      <c r="C157" t="s">
         <v>535</v>
       </c>
-      <c r="C157" t="s">
+      <c r="D157" t="s">
         <v>536</v>
       </c>
-      <c r="D157" t="s">
-        <v>537</v>
-      </c>
       <c r="E157" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F157" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
+        <v>537</v>
+      </c>
+      <c r="B158" t="s">
         <v>538</v>
       </c>
-      <c r="B158" t="s">
+      <c r="C158" t="s">
         <v>539</v>
       </c>
-      <c r="C158" t="s">
+      <c r="D158" t="s">
         <v>540</v>
       </c>
-      <c r="D158" t="s">
-        <v>541</v>
-      </c>
       <c r="E158" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F158" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
+        <v>541</v>
+      </c>
+      <c r="B159" t="s">
         <v>542</v>
       </c>
-      <c r="B159" t="s">
+      <c r="C159" t="s">
         <v>543</v>
       </c>
-      <c r="C159" t="s">
+      <c r="D159" t="s">
         <v>544</v>
       </c>
-      <c r="D159" t="s">
-        <v>545</v>
-      </c>
       <c r="E159" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F159" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
+        <v>545</v>
+      </c>
+      <c r="B160" t="s">
         <v>546</v>
       </c>
-      <c r="B160" t="s">
+      <c r="C160" t="s">
         <v>547</v>
       </c>
-      <c r="C160" t="s">
+      <c r="D160" t="s">
         <v>548</v>
       </c>
-      <c r="D160" t="s">
-        <v>549</v>
-      </c>
       <c r="E160" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F160" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
+        <v>549</v>
+      </c>
+      <c r="B161" t="s">
         <v>550</v>
       </c>
-      <c r="B161" t="s">
+      <c r="C161" t="s">
         <v>551</v>
       </c>
-      <c r="C161" t="s">
+      <c r="D161" t="s">
         <v>552</v>
       </c>
-      <c r="D161" t="s">
-        <v>553</v>
-      </c>
       <c r="E161" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F161" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
+        <v>553</v>
+      </c>
+      <c r="B162" t="s">
         <v>554</v>
       </c>
-      <c r="B162" t="s">
+      <c r="C162" t="s">
         <v>555</v>
       </c>
-      <c r="C162" t="s">
+      <c r="D162" t="s">
         <v>556</v>
       </c>
-      <c r="D162" t="s">
-        <v>557</v>
-      </c>
       <c r="E162" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F162" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
+        <v>557</v>
+      </c>
+      <c r="B163" t="s">
         <v>558</v>
       </c>
-      <c r="B163" t="s">
+      <c r="C163" t="s">
         <v>559</v>
       </c>
-      <c r="C163" t="s">
+      <c r="D163" t="s">
         <v>560</v>
       </c>
-      <c r="D163" t="s">
-        <v>561</v>
-      </c>
       <c r="E163" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F163" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
+        <v>561</v>
+      </c>
+      <c r="B164" t="s">
         <v>562</v>
       </c>
-      <c r="B164" t="s">
+      <c r="C164" t="s">
         <v>563</v>
       </c>
-      <c r="C164" t="s">
+      <c r="D164" t="s">
         <v>564</v>
       </c>
-      <c r="D164" t="s">
-        <v>565</v>
-      </c>
       <c r="E164" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F164" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
+        <v>565</v>
+      </c>
+      <c r="B165" t="s">
         <v>566</v>
       </c>
-      <c r="B165" t="s">
+      <c r="C165" t="s">
         <v>567</v>
       </c>
-      <c r="C165" t="s">
+      <c r="D165" t="s">
         <v>568</v>
       </c>
-      <c r="D165" t="s">
-        <v>569</v>
-      </c>
       <c r="E165" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F165" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
+        <v>569</v>
+      </c>
+      <c r="B166" t="s">
         <v>570</v>
       </c>
-      <c r="B166" t="s">
+      <c r="C166" t="s">
         <v>571</v>
       </c>
-      <c r="C166" t="s">
+      <c r="D166" t="s">
         <v>572</v>
       </c>
-      <c r="D166" t="s">
-        <v>573</v>
-      </c>
       <c r="E166" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F166" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
+        <v>573</v>
+      </c>
+      <c r="B167" t="s">
         <v>574</v>
       </c>
-      <c r="B167" t="s">
+      <c r="C167" t="s">
         <v>575</v>
       </c>
-      <c r="C167" t="s">
+      <c r="D167" t="s">
         <v>576</v>
       </c>
-      <c r="D167" t="s">
-        <v>577</v>
-      </c>
       <c r="E167" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F167" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
+        <v>577</v>
+      </c>
+      <c r="B168" t="s">
         <v>578</v>
       </c>
-      <c r="B168" t="s">
+      <c r="C168" t="s">
         <v>579</v>
-      </c>
-      <c r="C168" t="s">
-        <v>580</v>
       </c>
       <c r="D168" t="s">
         <v>271</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F168" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
+        <v>580</v>
+      </c>
+      <c r="B169" t="s">
         <v>581</v>
       </c>
-      <c r="B169" t="s">
+      <c r="C169" t="s">
         <v>582</v>
       </c>
-      <c r="C169" t="s">
+      <c r="D169" t="s">
         <v>583</v>
       </c>
-      <c r="D169" t="s">
-        <v>584</v>
-      </c>
       <c r="E169" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F169" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
+        <v>584</v>
+      </c>
+      <c r="B170" t="s">
         <v>585</v>
       </c>
-      <c r="B170" t="s">
+      <c r="C170" t="s">
         <v>586</v>
-      </c>
-      <c r="C170" t="s">
-        <v>587</v>
       </c>
       <c r="D170" t="s">
         <v>203</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F170" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
+        <v>587</v>
+      </c>
+      <c r="B171" t="s">
         <v>588</v>
-      </c>
-      <c r="B171" t="s">
-        <v>589</v>
       </c>
       <c r="C171" t="s">
         <v>281</v>
       </c>
       <c r="D171" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F171" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
+        <v>590</v>
+      </c>
+      <c r="B172" t="s">
         <v>591</v>
       </c>
-      <c r="B172" t="s">
+      <c r="C172" t="s">
         <v>592</v>
       </c>
-      <c r="C172" t="s">
+      <c r="D172" t="s">
         <v>593</v>
       </c>
-      <c r="D172" t="s">
-        <v>594</v>
-      </c>
       <c r="E172" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F172" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
+        <v>594</v>
+      </c>
+      <c r="B173" t="s">
         <v>595</v>
-      </c>
-      <c r="B173" t="s">
-        <v>596</v>
       </c>
       <c r="C173" t="s">
         <v>318</v>
       </c>
       <c r="D173" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F173" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
+        <v>597</v>
+      </c>
+      <c r="B174" t="s">
         <v>598</v>
       </c>
-      <c r="B174" t="s">
+      <c r="C174" t="s">
         <v>599</v>
       </c>
-      <c r="C174" t="s">
+      <c r="D174" t="s">
         <v>600</v>
       </c>
-      <c r="D174" t="s">
-        <v>601</v>
-      </c>
       <c r="E174" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F174" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
+        <v>601</v>
+      </c>
+      <c r="B175" t="s">
         <v>602</v>
       </c>
-      <c r="B175" t="s">
-        <v>603</v>
-      </c>
       <c r="C175" t="s">
+        <v>592</v>
+      </c>
+      <c r="D175" t="s">
         <v>593</v>
       </c>
-      <c r="D175" t="s">
-        <v>594</v>
-      </c>
       <c r="E175" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F175" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
+        <v>603</v>
+      </c>
+      <c r="B176" t="s">
         <v>604</v>
-      </c>
-      <c r="B176" t="s">
-        <v>605</v>
       </c>
       <c r="C176" t="s">
         <v>170</v>
@@ -6455,78 +6457,78 @@
         <v>93</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F176" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
+        <v>605</v>
+      </c>
+      <c r="B177" t="s">
         <v>606</v>
       </c>
-      <c r="B177" t="s">
+      <c r="C177" t="s">
         <v>607</v>
       </c>
-      <c r="C177" t="s">
+      <c r="D177" t="s">
         <v>608</v>
       </c>
-      <c r="D177" t="s">
-        <v>609</v>
-      </c>
       <c r="E177" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F177" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
+        <v>609</v>
+      </c>
+      <c r="B178" t="s">
         <v>610</v>
       </c>
-      <c r="B178" t="s">
+      <c r="C178" t="s">
         <v>611</v>
       </c>
-      <c r="C178" t="s">
+      <c r="D178" t="s">
         <v>612</v>
       </c>
-      <c r="D178" t="s">
-        <v>613</v>
-      </c>
       <c r="E178" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F178" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
+        <v>613</v>
+      </c>
+      <c r="B179" t="s">
         <v>614</v>
       </c>
-      <c r="B179" t="s">
+      <c r="C179" t="s">
         <v>615</v>
-      </c>
-      <c r="C179" t="s">
-        <v>616</v>
       </c>
       <c r="D179" t="s">
         <v>38</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F179" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
+        <v>616</v>
+      </c>
+      <c r="B180" t="s">
         <v>617</v>
-      </c>
-      <c r="B180" t="s">
-        <v>618</v>
       </c>
       <c r="C180" t="s">
         <v>15</v>
@@ -6535,58 +6537,58 @@
         <v>198</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F180" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
+        <v>618</v>
+      </c>
+      <c r="B181" t="s">
         <v>619</v>
       </c>
-      <c r="B181" t="s">
-        <v>620</v>
-      </c>
       <c r="C181" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D181" t="s">
         <v>134</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F181" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
+        <v>621</v>
+      </c>
+      <c r="B182" t="s">
         <v>622</v>
       </c>
-      <c r="B182" t="s">
+      <c r="C182" t="s">
         <v>623</v>
       </c>
-      <c r="C182" t="s">
+      <c r="D182" t="s">
         <v>624</v>
       </c>
-      <c r="D182" t="s">
-        <v>625</v>
-      </c>
       <c r="E182" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F182" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
+        <v>625</v>
+      </c>
+      <c r="B183" t="s">
         <v>626</v>
-      </c>
-      <c r="B183" t="s">
-        <v>627</v>
       </c>
       <c r="C183" t="s">
         <v>103</v>
@@ -6595,258 +6597,258 @@
         <v>276</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F183" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
+        <v>627</v>
+      </c>
+      <c r="B184" t="s">
         <v>628</v>
       </c>
-      <c r="B184" t="s">
+      <c r="C184" t="s">
         <v>629</v>
       </c>
-      <c r="C184" t="s">
+      <c r="D184" t="s">
         <v>630</v>
       </c>
-      <c r="D184" t="s">
-        <v>631</v>
-      </c>
       <c r="E184" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F184" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
+        <v>631</v>
+      </c>
+      <c r="B185" t="s">
         <v>632</v>
       </c>
-      <c r="B185" t="s">
+      <c r="C185" t="s">
         <v>633</v>
-      </c>
-      <c r="C185" t="s">
-        <v>634</v>
       </c>
       <c r="D185" t="s">
         <v>134</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F185" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
+        <v>634</v>
+      </c>
+      <c r="B186" t="s">
         <v>635</v>
       </c>
-      <c r="B186" t="s">
+      <c r="C186" t="s">
+        <v>509</v>
+      </c>
+      <c r="D186" t="s">
         <v>636</v>
       </c>
-      <c r="C186" t="s">
-        <v>510</v>
-      </c>
-      <c r="D186" t="s">
-        <v>637</v>
-      </c>
       <c r="E186" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F186" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
+        <v>637</v>
+      </c>
+      <c r="B187" t="s">
         <v>638</v>
       </c>
-      <c r="B187" t="s">
+      <c r="C187" t="s">
         <v>639</v>
-      </c>
-      <c r="C187" t="s">
-        <v>640</v>
       </c>
       <c r="D187" t="s">
         <v>185</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F187" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
+        <v>640</v>
+      </c>
+      <c r="B188" t="s">
         <v>641</v>
       </c>
-      <c r="B188" t="s">
+      <c r="C188" t="s">
         <v>642</v>
-      </c>
-      <c r="C188" t="s">
-        <v>643</v>
       </c>
       <c r="D188" t="s">
         <v>174</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F188" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
+        <v>643</v>
+      </c>
+      <c r="B189" t="s">
         <v>644</v>
       </c>
-      <c r="B189" t="s">
+      <c r="C189" t="s">
         <v>645</v>
       </c>
-      <c r="C189" t="s">
+      <c r="D189" t="s">
         <v>646</v>
       </c>
-      <c r="D189" t="s">
-        <v>647</v>
-      </c>
       <c r="E189" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F189" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
+        <v>647</v>
+      </c>
+      <c r="B190" t="s">
         <v>648</v>
-      </c>
-      <c r="B190" t="s">
-        <v>649</v>
       </c>
       <c r="C190" t="s">
         <v>106</v>
       </c>
       <c r="D190" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F190" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
+        <v>650</v>
+      </c>
+      <c r="B191" t="s">
         <v>651</v>
       </c>
-      <c r="B191" t="s">
+      <c r="C191" t="s">
+        <v>344</v>
+      </c>
+      <c r="D191" t="s">
         <v>652</v>
       </c>
-      <c r="C191" t="s">
-        <v>345</v>
-      </c>
-      <c r="D191" t="s">
-        <v>653</v>
-      </c>
       <c r="E191" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F191" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
+        <v>653</v>
+      </c>
+      <c r="B192" t="s">
         <v>654</v>
       </c>
-      <c r="B192" t="s">
-        <v>655</v>
-      </c>
       <c r="C192" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D192" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F192" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
+        <v>655</v>
+      </c>
+      <c r="B193" t="s">
         <v>656</v>
       </c>
-      <c r="B193" t="s">
+      <c r="C193" t="s">
         <v>657</v>
       </c>
-      <c r="C193" t="s">
-        <v>658</v>
-      </c>
       <c r="D193" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F193" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
+        <v>658</v>
+      </c>
+      <c r="B194" t="s">
         <v>659</v>
       </c>
-      <c r="B194" t="s">
+      <c r="C194" t="s">
         <v>660</v>
-      </c>
-      <c r="C194" t="s">
-        <v>661</v>
       </c>
       <c r="D194" t="s">
         <v>295</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F194" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
+        <v>662</v>
+      </c>
+      <c r="B195" t="s">
         <v>663</v>
       </c>
-      <c r="B195" t="s">
+      <c r="C195" t="s">
         <v>664</v>
       </c>
-      <c r="C195" t="s">
-        <v>665</v>
-      </c>
       <c r="D195" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F195" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
+        <v>665</v>
+      </c>
+      <c r="B196" t="s">
         <v>666</v>
-      </c>
-      <c r="B196" t="s">
-        <v>667</v>
       </c>
       <c r="C196" t="s">
         <v>10</v>
@@ -6855,18 +6857,18 @@
         <v>10</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F196" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
+        <v>667</v>
+      </c>
+      <c r="B197" t="s">
         <v>668</v>
-      </c>
-      <c r="B197" t="s">
-        <v>669</v>
       </c>
       <c r="C197" t="s">
         <v>184</v>
@@ -6875,18 +6877,18 @@
         <v>184</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F197" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
+        <v>669</v>
+      </c>
+      <c r="B198" t="s">
         <v>670</v>
-      </c>
-      <c r="B198" t="s">
-        <v>671</v>
       </c>
       <c r="C198" t="s">
         <v>213</v>
@@ -6895,18 +6897,18 @@
         <v>213</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F198" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
+        <v>671</v>
+      </c>
+      <c r="B199" t="s">
         <v>672</v>
-      </c>
-      <c r="B199" t="s">
-        <v>673</v>
       </c>
       <c r="C199" t="s">
         <v>23</v>
@@ -6915,98 +6917,98 @@
         <v>184</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F199" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
+        <v>673</v>
+      </c>
+      <c r="B200" t="s">
         <v>674</v>
       </c>
-      <c r="B200" t="s">
+      <c r="C200" t="s">
         <v>675</v>
       </c>
-      <c r="C200" t="s">
+      <c r="D200" t="s">
         <v>676</v>
       </c>
-      <c r="D200" t="s">
-        <v>677</v>
-      </c>
       <c r="E200" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F200" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
+        <v>677</v>
+      </c>
+      <c r="B201" t="s">
         <v>678</v>
       </c>
-      <c r="B201" t="s">
+      <c r="C201" t="s">
         <v>679</v>
       </c>
-      <c r="C201" t="s">
+      <c r="D201" t="s">
         <v>680</v>
       </c>
-      <c r="D201" t="s">
-        <v>681</v>
-      </c>
       <c r="E201" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F201" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
+        <v>681</v>
+      </c>
+      <c r="B202" t="s">
         <v>682</v>
       </c>
-      <c r="B202" t="s">
+      <c r="C202" t="s">
         <v>683</v>
-      </c>
-      <c r="C202" t="s">
-        <v>684</v>
       </c>
       <c r="D202" t="s">
         <v>156</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F202" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
+        <v>684</v>
+      </c>
+      <c r="B203" t="s">
         <v>685</v>
       </c>
-      <c r="B203" t="s">
+      <c r="C203" t="s">
+        <v>575</v>
+      </c>
+      <c r="D203" t="s">
         <v>686</v>
       </c>
-      <c r="C203" t="s">
-        <v>576</v>
-      </c>
-      <c r="D203" t="s">
-        <v>687</v>
-      </c>
       <c r="E203" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F203" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
+        <v>687</v>
+      </c>
+      <c r="B204" t="s">
         <v>688</v>
-      </c>
-      <c r="B204" t="s">
-        <v>689</v>
       </c>
       <c r="C204" t="s">
         <v>171</v>
@@ -7015,18 +7017,18 @@
         <v>117</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F204" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
+        <v>689</v>
+      </c>
+      <c r="B205" t="s">
         <v>690</v>
-      </c>
-      <c r="B205" t="s">
-        <v>691</v>
       </c>
       <c r="C205" t="s">
         <v>21</v>
@@ -7035,78 +7037,78 @@
         <v>50</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F205" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
+        <v>691</v>
+      </c>
+      <c r="B206" t="s">
         <v>692</v>
-      </c>
-      <c r="B206" t="s">
-        <v>693</v>
       </c>
       <c r="C206" t="s">
         <v>149</v>
       </c>
       <c r="D206" t="s">
+        <v>693</v>
+      </c>
+      <c r="E206" s="1" t="s">
         <v>694</v>
       </c>
-      <c r="E206" s="1" t="s">
-        <v>695</v>
-      </c>
       <c r="F206" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
+        <v>695</v>
+      </c>
+      <c r="B207" t="s">
         <v>696</v>
-      </c>
-      <c r="B207" t="s">
-        <v>697</v>
       </c>
       <c r="C207" t="s">
         <v>149</v>
       </c>
       <c r="D207" t="s">
+        <v>693</v>
+      </c>
+      <c r="E207" s="1" t="s">
         <v>694</v>
       </c>
-      <c r="E207" s="1" t="s">
-        <v>695</v>
-      </c>
       <c r="F207" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
+        <v>697</v>
+      </c>
+      <c r="B208" t="s">
         <v>698</v>
-      </c>
-      <c r="B208" t="s">
-        <v>699</v>
       </c>
       <c r="C208" t="s">
         <v>106</v>
       </c>
       <c r="D208" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="F208" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
+        <v>700</v>
+      </c>
+      <c r="B209" t="s">
         <v>701</v>
-      </c>
-      <c r="B209" t="s">
-        <v>702</v>
       </c>
       <c r="C209" t="s">
         <v>21</v>
@@ -7115,87 +7117,87 @@
         <v>276</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="F209" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
+        <v>702</v>
+      </c>
+      <c r="B210" t="s">
         <v>703</v>
       </c>
-      <c r="B210" t="s">
+      <c r="C210" t="s">
         <v>704</v>
-      </c>
-      <c r="C210" t="s">
-        <v>705</v>
       </c>
       <c r="D210" t="s">
         <v>16</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="F210" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
+        <v>705</v>
+      </c>
+      <c r="B211" t="s">
         <v>706</v>
       </c>
-      <c r="B211" t="s">
+      <c r="C211" t="s">
+        <v>657</v>
+      </c>
+      <c r="D211" t="s">
         <v>707</v>
       </c>
-      <c r="C211" t="s">
-        <v>658</v>
-      </c>
-      <c r="D211" t="s">
+      <c r="E211" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="E211" s="1" t="s">
-        <v>709</v>
-      </c>
       <c r="F211" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
+        <v>709</v>
+      </c>
+      <c r="B212" t="s">
         <v>710</v>
-      </c>
-      <c r="B212" t="s">
-        <v>711</v>
       </c>
       <c r="C212" t="s">
         <v>10</v>
       </c>
       <c r="D212" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="F212" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
+        <v>756</v>
+      </c>
+      <c r="B213" t="s">
+        <v>858</v>
+      </c>
+      <c r="C213" t="s">
         <v>757</v>
-      </c>
-      <c r="B213" t="s">
-        <v>859</v>
-      </c>
-      <c r="C213" t="s">
-        <v>758</v>
       </c>
       <c r="D213" t="s">
         <v>134</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="F213" t="s">
         <v>136</v>
@@ -7203,19 +7205,19 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
+        <v>759</v>
+      </c>
+      <c r="B214" t="s">
         <v>760</v>
       </c>
-      <c r="B214" t="s">
-        <v>761</v>
-      </c>
       <c r="C214" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="D214" t="s">
         <v>134</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="F214" t="s">
         <v>136</v>
@@ -7223,699 +7225,699 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
+        <v>761</v>
+      </c>
+      <c r="B215" t="s">
         <v>762</v>
       </c>
-      <c r="B215" t="s">
+      <c r="C215" t="s">
+        <v>571</v>
+      </c>
+      <c r="D215" t="s">
         <v>763</v>
       </c>
-      <c r="C215" t="s">
-        <v>572</v>
-      </c>
-      <c r="D215" t="s">
+      <c r="E215" s="1" t="s">
         <v>764</v>
       </c>
-      <c r="E215" s="1" t="s">
+      <c r="F215" t="s">
         <v>765</v>
-      </c>
-      <c r="F215" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B216" t="s">
+        <v>766</v>
+      </c>
+      <c r="C216" t="s">
         <v>767</v>
       </c>
-      <c r="C216" t="s">
+      <c r="D216" t="s">
         <v>768</v>
       </c>
-      <c r="D216" t="s">
-        <v>769</v>
-      </c>
       <c r="E216" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F216" t="s">
         <v>765</v>
-      </c>
-      <c r="F216" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B217" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C217" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D217" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E217" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F217" t="s">
         <v>765</v>
-      </c>
-      <c r="F217" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B218" t="s">
+        <v>770</v>
+      </c>
+      <c r="C218" t="s">
         <v>771</v>
       </c>
-      <c r="C218" t="s">
-        <v>772</v>
-      </c>
       <c r="D218" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E218" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F218" t="s">
         <v>765</v>
-      </c>
-      <c r="F218" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B219" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C219" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D219" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="E219" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F219" t="s">
         <v>765</v>
-      </c>
-      <c r="F219" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
+        <v>773</v>
+      </c>
+      <c r="B220" t="s">
         <v>774</v>
       </c>
-      <c r="B220" t="s">
+      <c r="C220" t="s">
         <v>775</v>
       </c>
-      <c r="C220" t="s">
+      <c r="D220" t="s">
         <v>776</v>
       </c>
-      <c r="D220" t="s">
-        <v>777</v>
-      </c>
       <c r="E220" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F220" t="s">
         <v>765</v>
-      </c>
-      <c r="F220" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B221" t="s">
+        <v>777</v>
+      </c>
+      <c r="C221" t="s">
         <v>778</v>
       </c>
-      <c r="C221" t="s">
+      <c r="D221" t="s">
         <v>779</v>
       </c>
-      <c r="D221" t="s">
-        <v>780</v>
-      </c>
       <c r="E221" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F221" t="s">
         <v>765</v>
-      </c>
-      <c r="F221" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B222" t="s">
+        <v>780</v>
+      </c>
+      <c r="C222" t="s">
         <v>781</v>
       </c>
-      <c r="C222" t="s">
+      <c r="D222" t="s">
         <v>782</v>
       </c>
-      <c r="D222" t="s">
-        <v>783</v>
-      </c>
       <c r="E222" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F222" t="s">
         <v>765</v>
-      </c>
-      <c r="F222" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B223" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C223" t="s">
+        <v>781</v>
+      </c>
+      <c r="D223" t="s">
         <v>782</v>
       </c>
-      <c r="D223" t="s">
-        <v>783</v>
-      </c>
       <c r="E223" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F223" t="s">
         <v>765</v>
-      </c>
-      <c r="F223" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B224" t="s">
+        <v>784</v>
+      </c>
+      <c r="C224" t="s">
         <v>785</v>
       </c>
-      <c r="C224" t="s">
+      <c r="D224" t="s">
         <v>786</v>
       </c>
-      <c r="D224" t="s">
-        <v>787</v>
-      </c>
       <c r="E224" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F224" t="s">
         <v>765</v>
-      </c>
-      <c r="F224" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B225" t="s">
+        <v>787</v>
+      </c>
+      <c r="C225" t="s">
         <v>788</v>
       </c>
-      <c r="C225" t="s">
+      <c r="D225" t="s">
         <v>789</v>
       </c>
-      <c r="D225" t="s">
-        <v>790</v>
-      </c>
       <c r="E225" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F225" t="s">
         <v>765</v>
-      </c>
-      <c r="F225" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B226" t="s">
+        <v>790</v>
+      </c>
+      <c r="C226" t="s">
         <v>791</v>
       </c>
-      <c r="C226" t="s">
+      <c r="D226" t="s">
         <v>792</v>
       </c>
-      <c r="D226" t="s">
-        <v>793</v>
-      </c>
       <c r="E226" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F226" t="s">
         <v>765</v>
-      </c>
-      <c r="F226" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B227" t="s">
+        <v>793</v>
+      </c>
+      <c r="C227" t="s">
         <v>794</v>
       </c>
-      <c r="C227" t="s">
+      <c r="D227" t="s">
         <v>795</v>
       </c>
-      <c r="D227" t="s">
-        <v>796</v>
-      </c>
       <c r="E227" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F227" t="s">
         <v>765</v>
-      </c>
-      <c r="F227" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B228" t="s">
+        <v>796</v>
+      </c>
+      <c r="C228" t="s">
         <v>797</v>
       </c>
-      <c r="C228" t="s">
-        <v>798</v>
-      </c>
       <c r="D228" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E228" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F228" t="s">
         <v>765</v>
-      </c>
-      <c r="F228" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B229" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C229" t="s">
+        <v>794</v>
+      </c>
+      <c r="D229" t="s">
         <v>795</v>
       </c>
-      <c r="D229" t="s">
-        <v>796</v>
-      </c>
       <c r="E229" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F229" t="s">
         <v>765</v>
-      </c>
-      <c r="F229" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B230" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C230" t="s">
+        <v>794</v>
+      </c>
+      <c r="D230" t="s">
         <v>795</v>
       </c>
-      <c r="D230" t="s">
-        <v>796</v>
-      </c>
       <c r="E230" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F230" t="s">
         <v>765</v>
-      </c>
-      <c r="F230" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
+        <v>800</v>
+      </c>
+      <c r="B231" t="s">
         <v>801</v>
       </c>
-      <c r="B231" t="s">
+      <c r="C231" t="s">
         <v>802</v>
       </c>
-      <c r="C231" t="s">
+      <c r="D231" t="s">
         <v>803</v>
       </c>
-      <c r="D231" t="s">
-        <v>804</v>
-      </c>
       <c r="E231" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F231" t="s">
         <v>765</v>
-      </c>
-      <c r="F231" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B232" t="s">
+        <v>804</v>
+      </c>
+      <c r="C232" t="s">
         <v>805</v>
       </c>
-      <c r="C232" t="s">
-        <v>806</v>
-      </c>
       <c r="D232" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E232" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F232" t="s">
         <v>765</v>
-      </c>
-      <c r="F232" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B233" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C233" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D233" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E233" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F233" t="s">
         <v>765</v>
-      </c>
-      <c r="F233" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B234" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C234" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D234" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E234" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F234" t="s">
         <v>765</v>
-      </c>
-      <c r="F234" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B235" t="s">
+        <v>808</v>
+      </c>
+      <c r="C235" t="s">
         <v>809</v>
       </c>
-      <c r="C235" t="s">
+      <c r="D235" t="s">
         <v>810</v>
       </c>
-      <c r="D235" t="s">
-        <v>811</v>
-      </c>
       <c r="E235" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F235" t="s">
         <v>765</v>
-      </c>
-      <c r="F235" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
+        <v>811</v>
+      </c>
+      <c r="B236" t="s">
         <v>812</v>
       </c>
-      <c r="B236" t="s">
+      <c r="C236" t="s">
         <v>813</v>
       </c>
-      <c r="C236" t="s">
+      <c r="D236" t="s">
         <v>814</v>
       </c>
-      <c r="D236" t="s">
+      <c r="E236" s="1" t="s">
         <v>815</v>
       </c>
-      <c r="E236" s="1" t="s">
-        <v>816</v>
-      </c>
       <c r="F236" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B237" t="s">
+        <v>816</v>
+      </c>
+      <c r="C237" t="s">
         <v>817</v>
       </c>
-      <c r="C237" t="s">
-        <v>818</v>
-      </c>
       <c r="D237" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="F237" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B238" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C238" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D238" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="F238" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B239" t="s">
+        <v>819</v>
+      </c>
+      <c r="C239" t="s">
         <v>820</v>
       </c>
-      <c r="C239" t="s">
-        <v>821</v>
-      </c>
       <c r="D239" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="F239" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B240" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C240" t="s">
+        <v>813</v>
+      </c>
+      <c r="D240" t="s">
         <v>814</v>
       </c>
-      <c r="D240" t="s">
+      <c r="E240" s="1" t="s">
         <v>815</v>
       </c>
-      <c r="E240" s="1" t="s">
-        <v>816</v>
-      </c>
       <c r="F240" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B241" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C241" t="s">
+        <v>813</v>
+      </c>
+      <c r="D241" t="s">
         <v>814</v>
       </c>
-      <c r="D241" t="s">
+      <c r="E241" s="1" t="s">
         <v>815</v>
       </c>
-      <c r="E241" s="1" t="s">
-        <v>816</v>
-      </c>
       <c r="F241" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B242" t="s">
+        <v>823</v>
+      </c>
+      <c r="C242" t="s">
         <v>824</v>
       </c>
-      <c r="C242" t="s">
-        <v>825</v>
-      </c>
       <c r="D242" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="F242" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B243" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C243" t="s">
+        <v>809</v>
+      </c>
+      <c r="D243" t="s">
         <v>810</v>
       </c>
-      <c r="D243" t="s">
-        <v>811</v>
-      </c>
       <c r="E243" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="F243" t="s">
         <v>765</v>
-      </c>
-      <c r="F243" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B244" t="s">
+        <v>826</v>
+      </c>
+      <c r="C244" t="s">
         <v>827</v>
       </c>
-      <c r="C244" t="s">
+      <c r="D244" t="s">
         <v>828</v>
       </c>
-      <c r="D244" t="s">
-        <v>829</v>
-      </c>
       <c r="E244" s="1" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="F244" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B245" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C245" t="s">
+        <v>813</v>
+      </c>
+      <c r="D245" t="s">
         <v>814</v>
       </c>
-      <c r="D245" t="s">
+      <c r="E245" s="1" t="s">
         <v>815</v>
       </c>
-      <c r="E245" s="1" t="s">
-        <v>816</v>
-      </c>
       <c r="F245" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B246" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C246" t="s">
+        <v>813</v>
+      </c>
+      <c r="D246" t="s">
         <v>814</v>
       </c>
-      <c r="D246" t="s">
+      <c r="E246" s="1" t="s">
         <v>815</v>
       </c>
-      <c r="E246" s="1" t="s">
-        <v>816</v>
-      </c>
       <c r="F246" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B247" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C247" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D247" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="F247" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B248" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C248" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D248" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="F248" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
+        <v>833</v>
+      </c>
+      <c r="B249" t="s">
         <v>834</v>
       </c>
-      <c r="B249" t="s">
+      <c r="C249" t="s">
         <v>835</v>
       </c>
-      <c r="C249" t="s">
+      <c r="D249" t="s">
         <v>836</v>
       </c>
-      <c r="D249" t="s">
+      <c r="E249" s="1" t="s">
         <v>837</v>
-      </c>
-      <c r="E249" s="1" t="s">
-        <v>838</v>
       </c>
       <c r="F249" t="s">
         <v>46</v>
@@ -7923,16 +7925,16 @@
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
+        <v>838</v>
+      </c>
+      <c r="B250" t="s">
         <v>839</v>
       </c>
-      <c r="B250" t="s">
+      <c r="C250" t="s">
         <v>840</v>
       </c>
-      <c r="C250" t="s">
+      <c r="D250" t="s">
         <v>841</v>
-      </c>
-      <c r="D250" t="s">
-        <v>842</v>
       </c>
       <c r="E250" s="1" t="s">
         <v>123</v>
@@ -7943,16 +7945,16 @@
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
+        <v>842</v>
+      </c>
+      <c r="B251" t="s">
         <v>843</v>
       </c>
-      <c r="B251" t="s">
+      <c r="C251" t="s">
         <v>844</v>
       </c>
-      <c r="C251" t="s">
+      <c r="D251" t="s">
         <v>845</v>
-      </c>
-      <c r="D251" t="s">
-        <v>846</v>
       </c>
       <c r="E251" s="1" t="s">
         <v>123</v>
@@ -7963,62 +7965,62 @@
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
+        <v>846</v>
+      </c>
+      <c r="B252" t="s">
         <v>847</v>
       </c>
-      <c r="B252" t="s">
+      <c r="C252" t="s">
         <v>848</v>
-      </c>
-      <c r="C252" t="s">
-        <v>849</v>
       </c>
       <c r="D252" t="s">
         <v>260</v>
       </c>
       <c r="E252" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="F252" t="s">
         <v>850</v>
-      </c>
-      <c r="F252" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
+        <v>851</v>
+      </c>
+      <c r="B253" t="s">
         <v>852</v>
       </c>
-      <c r="B253" t="s">
+      <c r="C253" t="s">
         <v>853</v>
-      </c>
-      <c r="C253" t="s">
-        <v>854</v>
       </c>
       <c r="D253" t="s">
         <v>260</v>
       </c>
       <c r="E253" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="F253" t="s">
         <v>850</v>
-      </c>
-      <c r="F253" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
+        <v>854</v>
+      </c>
+      <c r="B254" t="s">
         <v>855</v>
       </c>
-      <c r="B254" t="s">
+      <c r="C254" t="s">
         <v>856</v>
       </c>
-      <c r="C254" t="s">
+      <c r="D254" t="s">
         <v>857</v>
       </c>
-      <c r="D254" t="s">
-        <v>858</v>
-      </c>
       <c r="E254" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="F254" t="s">
         <v>850</v>
-      </c>
-      <c r="F254" t="s">
-        <v>851</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new APL NBS moorings
</commit_message>
<xml_diff>
--- a/data/buoys/Buoys_2023_04_01.xlsx
+++ b/data/buoys/Buoys_2023_04_01.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="861">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="867">
   <si>
     <t>N/A</t>
   </si>
@@ -2607,6 +2607,24 @@
   </si>
   <si>
     <t>59°54.747'N, 171°43.379’W</t>
+  </si>
+  <si>
+    <t>A3-23</t>
+  </si>
+  <si>
+    <t>A2-23</t>
+  </si>
+  <si>
+    <t>A4-23</t>
+  </si>
+  <si>
+    <t>66˚19.60’N, 168˚56.94’W</t>
+  </si>
+  <si>
+    <t>65˚46.86’N, 168˚34.06’W</t>
+  </si>
+  <si>
+    <t>65˚44.76’N, 168˚15.76’W</t>
   </si>
 </sst>
 </file>
@@ -2926,10 +2944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J254"/>
+  <dimension ref="A1:J257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="C239" workbookViewId="0">
+      <selection activeCell="F256" sqref="F256:F257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8023,6 +8041,57 @@
         <v>850</v>
       </c>
     </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A255" t="s">
+        <v>861</v>
+      </c>
+      <c r="B255" t="s">
+        <v>864</v>
+      </c>
+      <c r="C255" t="s">
+        <v>221</v>
+      </c>
+      <c r="D255" t="s">
+        <v>266</v>
+      </c>
+      <c r="F255" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A256" t="s">
+        <v>862</v>
+      </c>
+      <c r="B256" t="s">
+        <v>865</v>
+      </c>
+      <c r="C256" t="s">
+        <v>18</v>
+      </c>
+      <c r="D256" t="s">
+        <v>260</v>
+      </c>
+      <c r="F256" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A257" t="s">
+        <v>863</v>
+      </c>
+      <c r="B257" t="s">
+        <v>866</v>
+      </c>
+      <c r="C257" t="s">
+        <v>218</v>
+      </c>
+      <c r="D257" t="s">
+        <v>260</v>
+      </c>
+      <c r="F257" t="s">
+        <v>262</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>